<commit_message>
Adjusted MONDELEZDMIUS VTW point calc values for shelving racks and multiple clip strips
</commit_message>
<xml_diff>
--- a/Projects/MONDELEZDMIUS/Data/VTW_POINTS_SCORE.xlsx
+++ b/Projects/MONDELEZDMIUS/Data/VTW_POINTS_SCORE.xlsx
@@ -164,13 +164,12 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.1071428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -258,7 +257,8 @@
         <v>11</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>4</v>
+        <f aca="false">4*4</f>
+        <v>16</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -282,7 +282,8 @@
         <v>14</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>2</v>
+        <f aca="false">2*4</f>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>